<commit_message>
Cambios a Plan de Trabajo
</commit_message>
<xml_diff>
--- a/Documentos/Plan de Trabajo ASN.xlsx
+++ b/Documentos/Plan de Trabajo ASN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\ASN\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418B61E0-238C-48C6-AB8F-DE014933126E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F3E01D-2E83-4941-AE10-50AE75A7AB6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E673171D-683B-4146-8516-79FB6088E25E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="118">
   <si>
     <t>Artefacto</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>ABC Conceptos de Nómina, Montos y %</t>
-  </si>
-  <si>
-    <t>ABC y desactivación de nómina por país</t>
   </si>
   <si>
     <t>5.3.5</t>
@@ -843,6 +840,9 @@
 Se requiere definir los archivos para Data Analysis</t>
   </si>
   <si>
+    <t>5.5.5</t>
+  </si>
+  <si>
     <t>Se requiere definición</t>
   </si>
   <si>
@@ -851,6 +851,30 @@
   <si>
     <t>Definir cuales pantallas se consultarán desde smartphone.
 Aplicar Bootstrap a estas pantallas.</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Confirmar si se requiere un formato de configuración o si se realizará una configuración inicial.</t>
+  </si>
+  <si>
+    <t>5.1.</t>
+  </si>
+  <si>
+    <t>Se requiere definición de layouts.</t>
+  </si>
+  <si>
+    <t>Nomina, Sistemas</t>
+  </si>
+  <si>
+    <t>Se requiere definición. Definición de momento en que se aprueba automáticamente la solicitud.</t>
+  </si>
+  <si>
+    <t>ABC y desactivación de motivos de solicitud</t>
+  </si>
+  <si>
+    <t>ABC y desactivación de conceptos de nómina por país</t>
   </si>
 </sst>
 </file>
@@ -873,12 +897,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -893,8 +923,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -904,11 +935,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1218,11 +1275,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F6DE5-E41E-471A-AEDE-F42525837133}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1236,7 +1291,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
@@ -1252,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1269,21 +1324,22 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>46</v>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1297,7 +1353,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1305,13 +1361,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1325,7 +1381,7 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,49 +1389,50 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="A8" s="6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
-        <v>18</v>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -1386,134 +1443,148 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>45</v>
+      <c r="B23" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1525,402 +1596,491 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F824BD43-B57F-4E21-B61F-FCFB9295D04B}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="98.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="33" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="E21" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B23" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="B24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="B25" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="B26" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B27" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="B28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="B29" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="B30" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="B31" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="B32" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="B33" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="B34" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="B35" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="B36" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="B37" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="B38" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="B39" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="B40" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="B41" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:E42">
+    <cfRule type="containsBlanks" dxfId="0" priority="3">
+      <formula>LEN(TRIM(C2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización de documentos y documentación de Prototipos
</commit_message>
<xml_diff>
--- a/Documentos/Plan de Trabajo ASN.xlsx
+++ b/Documentos/Plan de Trabajo ASN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\ASN\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E7B3D1-EA9A-46EF-84AB-71641F2C631C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7806DE-0665-432A-A889-9C3023A1B91E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E673171D-683B-4146-8516-79FB6088E25E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{E673171D-683B-4146-8516-79FB6088E25E}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Trabajo General" sheetId="3" r:id="rId1"/>
@@ -1410,14 +1410,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1850,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F6DE5-E41E-471A-AEDE-F42525837133}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2482,12 +2475,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:J23">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(I2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:L23">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2500,7 +2493,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F824BD43-B57F-4E21-B61F-FCFB9295D04B}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E18" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3325,7 +3320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF37CD87-CEDF-44DC-B92D-938F2F5925C5}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>